<commit_message>
Fix duplicated when updates detected
</commit_message>
<xml_diff>
--- a/Datos/Usuarios_General.xlsx
+++ b/Datos/Usuarios_General.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\dev\Sergio_Tejeda\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\dev\DietGenerator\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F5773C-F734-471D-825F-C30FDEC49633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851A292F-FB86-4F80-B4E4-F08D6AD668B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>